<commit_message>
-> Scripting DPLKINV101-001 until DPLKINV105-001 (Setup Tipe Transaksi Fixed Income) -> Scripting DPLKINV106-001 until DPLKINV110-001 (Profile Fixed Income) -> Scripting DPLKINV111-001 until DPLKINV115-001 (Setup Tipe Transaksi Reksadana) -> Scripting DPLKINV116-001 until DPLKINV120-001 (Jenis Porto Reksadana)
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKINV101-001 -  Tipe Transaksi Investasi - Fixed Income Tambah Data.xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKINV101-001 -  Tipe Transaksi Investasi - Fixed Income Tambah Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DPLK\Lib_Repo_Excel\FileExcel_DPLK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF76B1F-1FFC-48D6-9D31-FDA7EB43354A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308B01A4-5FDD-4BCE-847A-61B82D6E3565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -511,7 +511,7 @@
   <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,7 +530,7 @@
     <col min="12" max="12" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="22.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="6.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="10.28515625" style="1" bestFit="1" customWidth="1"/>

</xml_diff>